<commit_message>
Added 3 APIs-Heartbeat, logoff, session
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/clientCode.xlsx
+++ b/BloodstreamAPI/testData/clientCode.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FB4414-7CEE-4AD3-A8EC-7EBBF7C5908E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{34E8BC20-AA84-461B-B064-924F92B45353}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="5745" tabRatio="715" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getAssays" sheetId="8" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="putClientSites" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="7">
   <si>
     <t>EndPoint</t>
   </si>
@@ -408,7 +409,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,9 +449,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -461,18 +460,14 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -522,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB169F1-53FF-41E3-B017-C1DD1689979C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,9 +558,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -576,18 +569,14 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -638,7 +627,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,9 +667,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -691,18 +678,14 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -982,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B58CB45-E23F-4A4F-9C6B-BCED5E8044BA}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added around 4-6 Drop 2 defects test cases
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/clientCode.xlsx
+++ b/BloodstreamAPI/testData/clientCode.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FBD5E7-B723-4E9F-806D-A93F0BCC3CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9C1EF6A2-EE79-4FF9-A8F4-98FA1777CA53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="5745" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getAssays" sheetId="8" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="putClientSites" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,12 +409,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -422,7 +423,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -430,7 +431,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -438,71 +439,52 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
+    </row>
+    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -510,15 +492,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB169F1-53FF-41E3-B017-C1DD1689979C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -527,7 +509,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -535,7 +517,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -543,71 +525,53 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
+    </row>
+    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -615,15 +579,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E94795B-07F7-4F5F-BA6C-70D17F751F3E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -632,7 +596,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -640,7 +604,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -648,21 +612,21 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -671,7 +635,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -679,7 +643,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -687,6 +651,9 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
+    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
@@ -704,9 +671,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -715,7 +682,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -723,7 +690,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -731,14 +698,14 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -747,7 +714,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -755,7 +722,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -763,14 +730,14 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -779,7 +746,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -787,7 +754,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,9 +780,9 @@
       <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -824,7 +791,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -832,7 +799,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -840,14 +807,14 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -856,7 +823,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -864,7 +831,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -872,14 +839,14 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -888,7 +855,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -896,7 +863,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -922,9 +889,9 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -933,7 +900,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -941,7 +908,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -949,14 +916,14 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -965,7 +932,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -973,7 +940,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -981,14 +948,14 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -997,7 +964,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +972,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Pushed drop 3 test cases and some dry run defects
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/clientCode.xlsx
+++ b/BloodstreamAPI/testData/clientCode.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{749473C6-C953-4A02-95AE-84D848A9F718}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE78BA4E-AD1B-4497-A669-4341D80AFA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getAssays" sheetId="8" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <sheet name="putClientSites" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M27"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
   <si>
     <t>EndPoint</t>
   </si>
@@ -47,6 +46,9 @@
   </si>
   <si>
     <t>/configuration/clientCode/clientSites</t>
+  </si>
+  <si>
+    <t>Assert409</t>
   </si>
 </sst>
 </file>
@@ -438,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70C48DD-C9F7-4E07-93E4-989CB3728A5F}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -517,14 +519,6 @@
       <c r="D8" s="12"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -532,7 +526,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB169F1-53FF-41E3-B017-C1DD1689979C}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -610,10 +604,6 @@
       <c r="D8" s="12"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -621,9 +611,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E94795B-07F7-4F5F-BA6C-70D17F751F3E}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -632,54 +622,42 @@
     <col min="1" max="1" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -687,10 +665,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDD8A9B-A86D-4451-AA0A-6B485F7CCB08}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,11 +762,39 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -796,10 +802,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADCA34D-4993-4197-B420-9E2D0548D35B}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,11 +899,39 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -905,10 +939,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B58CB45-E23F-4A4F-9C6B-BCED5E8044BA}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,11 +1036,39 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>